<commit_message>
tidy away address code into functions
</commit_message>
<xml_diff>
--- a/excel_example.xlsx
+++ b/excel_example.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Address</t>
   </si>
@@ -49,42 +49,6 @@
   </si>
   <si>
     <t>Huntington Station</t>
-  </si>
-  <si>
-    <t>9553 Carousel Center Drive</t>
-  </si>
-  <si>
-    <t>Syracuse</t>
-  </si>
-  <si>
-    <t>2655 Richmond Ave</t>
-  </si>
-  <si>
-    <t>Staten Island</t>
-  </si>
-  <si>
-    <t>7979 Victor Road</t>
-  </si>
-  <si>
-    <t>Victor</t>
-  </si>
-  <si>
-    <t>1591 Palisades Center Drive</t>
-  </si>
-  <si>
-    <t>West Nyack</t>
-  </si>
-  <si>
-    <t>125 Westchester Ave.</t>
-  </si>
-  <si>
-    <t>White Plains</t>
-  </si>
-  <si>
-    <t>103 Prince Street</t>
-  </si>
-  <si>
-    <t>New York</t>
   </si>
 </sst>
 </file>
@@ -130,7 +94,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -153,13 +117,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -167,6 +193,24 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -334,13 +378,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -430,19 +468,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -697,13 +735,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1007,19 +1039,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1270,7 +1302,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1278,7 +1310,8 @@
   <cols>
     <col min="1" max="1" width="27.3516" style="1" customWidth="1"/>
     <col min="2" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="256" width="11.8516" style="1" customWidth="1"/>
+    <col min="4" max="5" width="11.8516" style="1" customWidth="1"/>
+    <col min="6" max="256" width="11.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1291,6 +1324,8 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1302,6 +1337,8 @@
       <c r="C2" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -1313,6 +1350,8 @@
       <c r="C3" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -1324,6 +1363,8 @@
       <c r="C4" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" t="s" s="2">
@@ -1335,72 +1376,50 @@
       <c r="C5" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>5</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>5</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>5</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>5</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>5</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>5</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -1420,79 +1439,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="3" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="3" customWidth="1"/>
+    <col min="1" max="5" width="11.5" style="9" customWidth="1"/>
+    <col min="6" max="256" width="11.8516" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -1512,79 +1531,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="5" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="5" customWidth="1"/>
+    <col min="1" max="5" width="11.5" style="11" customWidth="1"/>
+    <col min="6" max="256" width="11.8516" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
script merges coord results with worksheet and writes to a new file
</commit_message>
<xml_diff>
--- a/excel_example.xlsx
+++ b/excel_example.xlsx
@@ -13,42 +13,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
   </si>
   <si>
     <t>1 Crossgates Mall Road</t>
   </si>
   <si>
-    <t>Albany</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
     <t>Duke Rd &amp; Walden Ave</t>
-  </si>
-  <si>
-    <t>Buffalo</t>
   </si>
   <si>
     <t>630 Old Country Rd.</t>
   </si>
   <si>
-    <t>Garden City</t>
-  </si>
-  <si>
     <t>160 Walt Whitman Rd.</t>
-  </si>
-  <si>
-    <t>Huntington Station</t>
   </si>
 </sst>
 </file>
@@ -94,7 +73,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,75 +96,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -193,24 +110,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1302,124 +1201,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="27.3516" style="1" customWidth="1"/>
-    <col min="2" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="5" width="11.8516" style="1" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="1" customWidth="1"/>
+    <col min="2" max="256" width="11.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="2">
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="2">
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -1439,79 +1254,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="9" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="9" customWidth="1"/>
+    <col min="1" max="5" width="11.5" style="3" customWidth="1"/>
+    <col min="6" max="256" width="11.8516" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -1531,79 +1346,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="11" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="11" customWidth="1"/>
+    <col min="1" max="5" width="11.5" style="5" customWidth="1"/>
+    <col min="6" max="256" width="11.8516" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added logging to script console output
</commit_message>
<xml_diff>
--- a/excel_example.xlsx
+++ b/excel_example.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>Address</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>160 Walt Whitman Rd.</t>
+  </si>
+  <si>
+    <t>Matrix house Milton Keynes UK</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1204,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1235,6 +1238,81 @@
       <c r="A5" t="s" s="2">
         <v>4</v>
       </c>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" t="s" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" t="s" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" t="s" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" t="s" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="13.65" customHeight="1">
+      <c r="A11" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" ht="13.65" customHeight="1">
+      <c r="A12" t="s" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" ht="13.65" customHeight="1">
+      <c r="A13" t="s" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" ht="13.65" customHeight="1">
+      <c r="A14" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" ht="13.65" customHeight="1">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" ht="13.65" customHeight="1">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" ht="13.65" customHeight="1">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" ht="13.65" customHeight="1">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" ht="13.65" customHeight="1">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" ht="13.65" customHeight="1">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" ht="13.65" customHeight="1">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" ht="13.65" customHeight="1">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" ht="13.65" customHeight="1">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" ht="13.65" customHeight="1">
+      <c r="A24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>

</xml_diff>